<commit_message>
feat(Network Arch.xlsx): Add time overhead of SYA shifting
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云网络结构分析.xlsx
+++ b/hardware/docs/01-top/点云网络结构分析.xlsx
@@ -550,7 +550,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="156">
   <si>
     <t>Layer</t>
   </si>
@@ -4346,6 +4346,91 @@
   </si>
   <si>
     <t>MLP-Only Weight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>SYA sift</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>导致增大的计算时间</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>最差情况</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NUM_ROW=32</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>最好情况</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NUM_ROW=16</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>修改</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>SYA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1x16, NUM_ROW=8</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5035,18 +5120,66 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5065,59 +5198,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5399,11 +5484,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT46"/>
+  <dimension ref="A1:AX46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
+      <selection pane="bottomLeft" activeCell="AX2" sqref="AX2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5439,29 +5524,32 @@
     <col min="41" max="41" width="25.109375" style="3" customWidth="1"/>
     <col min="42" max="42" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="43" max="45" width="12.6640625" style="65" customWidth="1"/>
-    <col min="46" max="16384" width="8.88671875" style="3"/>
+    <col min="46" max="47" width="8.88671875" style="3"/>
+    <col min="48" max="49" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="51" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="70.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:50" ht="70.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="103" t="s">
+      <c r="B1" s="101"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="104"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="103" t="s">
+      <c r="E1" s="119"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="104"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="103" t="s">
+      <c r="H1" s="119"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="105"/>
+      <c r="K1" s="97"/>
       <c r="L1" s="4" t="s">
         <v>36</v>
       </c>
@@ -5477,9 +5565,9 @@
       <c r="P1" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="93"/>
-      <c r="R1" s="93"/>
-      <c r="S1" s="94"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="93"/>
       <c r="T1" s="7" t="s">
         <v>37</v>
       </c>
@@ -5493,45 +5581,49 @@
       <c r="X1" s="52"/>
       <c r="Y1" s="52"/>
       <c r="Z1" s="52"/>
-      <c r="AA1" s="118" t="s">
+      <c r="AA1" s="109" t="s">
         <v>118</v>
       </c>
-      <c r="AB1" s="119"/>
-      <c r="AC1" s="119"/>
-      <c r="AD1" s="119"/>
-      <c r="AE1" s="119"/>
-      <c r="AF1" s="120"/>
-      <c r="AG1" s="115" t="s">
+      <c r="AB1" s="110"/>
+      <c r="AC1" s="110"/>
+      <c r="AD1" s="110"/>
+      <c r="AE1" s="110"/>
+      <c r="AF1" s="111"/>
+      <c r="AG1" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="AH1" s="116"/>
-      <c r="AI1" s="117"/>
-      <c r="AJ1" s="115" t="s">
+      <c r="AH1" s="107"/>
+      <c r="AI1" s="108"/>
+      <c r="AJ1" s="106" t="s">
         <v>115</v>
       </c>
-      <c r="AK1" s="116"/>
-      <c r="AL1" s="116" t="s">
+      <c r="AK1" s="107"/>
+      <c r="AL1" s="107" t="s">
         <v>111</v>
       </c>
-      <c r="AM1" s="116"/>
-      <c r="AN1" s="117"/>
+      <c r="AM1" s="107"/>
+      <c r="AN1" s="108"/>
       <c r="AO1" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="AP1" s="94"/>
+      <c r="AP1" s="93"/>
       <c r="AQ1" s="92" t="s">
         <v>104</v>
       </c>
-      <c r="AR1" s="93"/>
-      <c r="AS1" s="94"/>
+      <c r="AR1" s="98"/>
+      <c r="AS1" s="93"/>
       <c r="AT1" s="70" t="s">
         <v>99</v>
       </c>
+      <c r="AV1" s="96" t="s">
+        <v>152</v>
+      </c>
+      <c r="AW1" s="97"/>
     </row>
-    <row r="2" spans="1:46" s="8" customFormat="1" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="112"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="114"/>
+    <row r="2" spans="1:50" s="8" customFormat="1" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="103"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="105"/>
       <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
@@ -5650,12 +5742,21 @@
       <c r="AS2" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AV2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AX2" s="8" t="s">
+        <v>155</v>
+      </c>
     </row>
-    <row r="3" spans="1:46" s="42" customFormat="1" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="101" t="s">
+    <row r="3" spans="1:50" s="42" customFormat="1" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="102"/>
+      <c r="B3" s="118"/>
       <c r="C3" s="42" t="s">
         <v>14</v>
       </c>
@@ -5753,12 +5854,24 @@
         <f>(M3/2+N3)/AI3*1024*8</f>
         <v>51</v>
       </c>
+      <c r="AV3" s="42">
+        <f>Q3/(F3/(F3+16))</f>
+        <v>608</v>
+      </c>
+      <c r="AW3" s="42">
+        <f>Q3/(F3/(F3+32))</f>
+        <v>1120</v>
+      </c>
+      <c r="AX3" s="42">
+        <f>Q3/(F3/(F3+8))</f>
+        <v>352</v>
+      </c>
     </row>
-    <row r="4" spans="1:46" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="106" t="s">
+    <row r="4" spans="1:50" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="109" t="s">
+      <c r="B4" s="95" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -5853,10 +5966,18 @@
       <c r="AQ4" s="68"/>
       <c r="AR4" s="74"/>
       <c r="AS4" s="74"/>
+      <c r="AW4" s="42">
+        <f t="shared" ref="AW4:AW37" si="4">Q4/(F4/(F4+32))</f>
+        <v>0</v>
+      </c>
+      <c r="AX4" s="42">
+        <f t="shared" ref="AX4:AX37" si="5">Q4/(F4/(F4+8))</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:46" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="106"/>
-      <c r="B5" s="109"/>
+    <row r="5" spans="1:50" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="112"/>
+      <c r="B5" s="95"/>
       <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
@@ -5955,10 +6076,18 @@
         <v>6.4</v>
       </c>
       <c r="AS5" s="71"/>
+      <c r="AW5" s="42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AX5" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:46" s="20" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="107"/>
-      <c r="B6" s="107" t="s">
+    <row r="6" spans="1:50" s="20" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="94"/>
+      <c r="B6" s="94" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="20" t="s">
@@ -6074,11 +6203,23 @@
         <f>AQ5</f>
         <v>12</v>
       </c>
+      <c r="AV6" s="42">
+        <f>Q6/(F6/(F6+16))</f>
+        <v>1536</v>
+      </c>
+      <c r="AW6" s="42">
+        <f t="shared" si="4"/>
+        <v>2048</v>
+      </c>
+      <c r="AX6" s="42">
+        <f t="shared" si="5"/>
+        <v>1280</v>
+      </c>
     </row>
-    <row r="7" spans="1:46" s="20" customFormat="1" ht="85.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="107"/>
-      <c r="B7" s="107"/>
-      <c r="C7" s="107" t="s">
+    <row r="7" spans="1:50" s="20" customFormat="1" ht="71.400000000000006" x14ac:dyDescent="0.25">
+      <c r="A7" s="94"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="20">
@@ -6182,11 +6323,23 @@
       <c r="AQ7" s="66"/>
       <c r="AR7" s="66"/>
       <c r="AS7" s="66"/>
+      <c r="AV7" s="42">
+        <f>Q7/(F7/(F7+16))</f>
+        <v>640</v>
+      </c>
+      <c r="AW7" s="42">
+        <f t="shared" si="4"/>
+        <v>768</v>
+      </c>
+      <c r="AX7" s="42">
+        <f t="shared" si="5"/>
+        <v>576</v>
+      </c>
     </row>
-    <row r="8" spans="1:46" s="20" customFormat="1" ht="57" x14ac:dyDescent="0.25">
-      <c r="A8" s="107"/>
-      <c r="B8" s="107"/>
-      <c r="C8" s="107"/>
+    <row r="8" spans="1:50" s="20" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A8" s="94"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="94"/>
       <c r="D8" s="20">
         <v>512</v>
       </c>
@@ -6287,9 +6440,21 @@
       <c r="AQ8" s="66"/>
       <c r="AR8" s="66"/>
       <c r="AS8" s="66"/>
+      <c r="AV8" s="42">
+        <f>Q8/(F8/(F8+16))</f>
+        <v>1024</v>
+      </c>
+      <c r="AW8" s="42">
+        <f t="shared" si="4"/>
+        <v>1536</v>
+      </c>
+      <c r="AX8" s="42">
+        <f t="shared" si="5"/>
+        <v>768</v>
+      </c>
     </row>
-    <row r="9" spans="1:46" s="30" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="106"/>
+    <row r="9" spans="1:50" s="30" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A9" s="112"/>
       <c r="B9" s="30" t="s">
         <v>16</v>
       </c>
@@ -6318,13 +6483,21 @@
       <c r="M9" s="32"/>
       <c r="N9" s="33"/>
       <c r="O9" s="32"/>
+      <c r="AW9" s="42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AX9" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:46" s="24" customFormat="1" ht="42" x14ac:dyDescent="0.25">
-      <c r="A10" s="108"/>
-      <c r="B10" s="108" t="s">
+    <row r="10" spans="1:50" s="24" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="A10" s="99"/>
+      <c r="B10" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="108" t="s">
+      <c r="C10" s="99" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="24">
@@ -6423,11 +6596,23 @@
       <c r="AQ10" s="67"/>
       <c r="AR10" s="67"/>
       <c r="AS10" s="67"/>
+      <c r="AV10" s="42">
+        <f>Q10/(F10/(F10+16))</f>
+        <v>640</v>
+      </c>
+      <c r="AW10" s="42">
+        <f t="shared" si="4"/>
+        <v>768</v>
+      </c>
+      <c r="AX10" s="42">
+        <f t="shared" si="5"/>
+        <v>576</v>
+      </c>
     </row>
-    <row r="11" spans="1:46" s="24" customFormat="1" ht="84.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="108"/>
-      <c r="B11" s="108"/>
-      <c r="C11" s="108"/>
+    <row r="11" spans="1:50" s="24" customFormat="1" ht="84.6" x14ac:dyDescent="0.25">
+      <c r="A11" s="99"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="99"/>
       <c r="D11" s="24">
         <v>512</v>
       </c>
@@ -6520,12 +6705,24 @@
       <c r="AQ11" s="67"/>
       <c r="AR11" s="67"/>
       <c r="AS11" s="67"/>
+      <c r="AV11" s="42">
+        <f>Q11/(F11/(F11+16))</f>
+        <v>1024</v>
+      </c>
+      <c r="AW11" s="42">
+        <f t="shared" si="4"/>
+        <v>1536</v>
+      </c>
+      <c r="AX11" s="42">
+        <f t="shared" si="5"/>
+        <v>768</v>
+      </c>
     </row>
-    <row r="12" spans="1:46" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="106" t="s">
+    <row r="12" spans="1:50" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="109" t="s">
+      <c r="B12" s="95" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -6609,10 +6806,18 @@
       <c r="AQ12" s="68"/>
       <c r="AR12" s="68"/>
       <c r="AS12" s="68"/>
+      <c r="AW12" s="42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AX12" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:46" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="106"/>
-      <c r="B13" s="109"/>
+    <row r="13" spans="1:50" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="112"/>
+      <c r="B13" s="95"/>
       <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
@@ -6696,10 +6901,18 @@
       </c>
       <c r="AR13" s="68"/>
       <c r="AS13" s="68"/>
+      <c r="AW13" s="42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AX13" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:46" s="20" customFormat="1" ht="86.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="107"/>
-      <c r="B14" s="107" t="s">
+    <row r="14" spans="1:50" s="20" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A14" s="94"/>
+      <c r="B14" s="94" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="20" t="s">
@@ -6796,11 +7009,23 @@
       <c r="AQ14" s="66"/>
       <c r="AR14" s="66"/>
       <c r="AS14" s="66"/>
+      <c r="AV14" s="42">
+        <f>Q14/(F14/(F14+16))</f>
+        <v>2560</v>
+      </c>
+      <c r="AW14" s="42">
+        <f t="shared" si="4"/>
+        <v>3072</v>
+      </c>
+      <c r="AX14" s="42">
+        <f t="shared" si="5"/>
+        <v>2304</v>
+      </c>
     </row>
-    <row r="15" spans="1:46" s="20" customFormat="1" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="107"/>
-      <c r="B15" s="107"/>
-      <c r="C15" s="107" t="s">
+    <row r="15" spans="1:50" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="94"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="20">
@@ -6890,11 +7115,23 @@
       <c r="AQ15" s="66"/>
       <c r="AR15" s="66"/>
       <c r="AS15" s="66"/>
+      <c r="AV15" s="42">
+        <f>Q15/(F15/(F15+16))</f>
+        <v>1152</v>
+      </c>
+      <c r="AW15" s="42">
+        <f t="shared" si="4"/>
+        <v>1280</v>
+      </c>
+      <c r="AX15" s="42">
+        <f t="shared" si="5"/>
+        <v>1088</v>
+      </c>
     </row>
-    <row r="16" spans="1:46" s="20" customFormat="1" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="107"/>
-      <c r="B16" s="107"/>
-      <c r="C16" s="107"/>
+    <row r="16" spans="1:50" s="20" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="94"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="94"/>
       <c r="D16" s="20">
         <v>256</v>
       </c>
@@ -6982,9 +7219,21 @@
       <c r="AQ16" s="66"/>
       <c r="AR16" s="66"/>
       <c r="AS16" s="66"/>
+      <c r="AV16" s="42">
+        <f>Q16/(F16/(F16+16))</f>
+        <v>1536</v>
+      </c>
+      <c r="AW16" s="42">
+        <f t="shared" si="4"/>
+        <v>2048</v>
+      </c>
+      <c r="AX16" s="42">
+        <f t="shared" si="5"/>
+        <v>1280</v>
+      </c>
     </row>
-    <row r="17" spans="1:45" s="30" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="106"/>
+    <row r="17" spans="1:50" s="30" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="112"/>
       <c r="B17" s="30" t="s">
         <v>16</v>
       </c>
@@ -7013,13 +7262,21 @@
       <c r="M17" s="32"/>
       <c r="N17" s="33"/>
       <c r="O17" s="32"/>
+      <c r="AW17" s="42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AX17" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:45" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="108"/>
-      <c r="B18" s="108" t="s">
+    <row r="18" spans="1:50" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="99"/>
+      <c r="B18" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="108" t="s">
+      <c r="C18" s="99" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="24">
@@ -7104,11 +7361,23 @@
       <c r="AQ18" s="67"/>
       <c r="AR18" s="67"/>
       <c r="AS18" s="67"/>
+      <c r="AV18" s="42">
+        <f>Q18/(F18/(F18+16))</f>
+        <v>1152</v>
+      </c>
+      <c r="AW18" s="42">
+        <f t="shared" si="4"/>
+        <v>1280</v>
+      </c>
+      <c r="AX18" s="42">
+        <f t="shared" si="5"/>
+        <v>1088</v>
+      </c>
     </row>
-    <row r="19" spans="1:45" s="24" customFormat="1" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="108"/>
-      <c r="B19" s="108"/>
-      <c r="C19" s="108"/>
+    <row r="19" spans="1:50" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="99"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="99"/>
       <c r="D19" s="24">
         <v>256</v>
       </c>
@@ -7191,12 +7460,24 @@
       <c r="AQ19" s="67"/>
       <c r="AR19" s="67"/>
       <c r="AS19" s="67"/>
+      <c r="AV19" s="42">
+        <f>Q19/(F19/(F19+16))</f>
+        <v>1536</v>
+      </c>
+      <c r="AW19" s="42">
+        <f t="shared" si="4"/>
+        <v>2048</v>
+      </c>
+      <c r="AX19" s="42">
+        <f t="shared" si="5"/>
+        <v>1280</v>
+      </c>
     </row>
-    <row r="20" spans="1:45" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="106" t="s">
+    <row r="20" spans="1:50" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="109" t="s">
+      <c r="B20" s="95" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="13" t="s">
@@ -7280,10 +7561,18 @@
       <c r="AQ20" s="68"/>
       <c r="AR20" s="68"/>
       <c r="AS20" s="68"/>
+      <c r="AW20" s="42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AX20" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:45" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="106"/>
-      <c r="B21" s="109"/>
+    <row r="21" spans="1:50" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="112"/>
+      <c r="B21" s="95"/>
       <c r="C21" s="13" t="s">
         <v>12</v>
       </c>
@@ -7367,10 +7656,18 @@
       </c>
       <c r="AR21" s="68"/>
       <c r="AS21" s="68"/>
+      <c r="AW21" s="42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AX21" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:45" s="20" customFormat="1" ht="71.400000000000006" x14ac:dyDescent="0.25">
-      <c r="A22" s="107"/>
-      <c r="B22" s="107" t="s">
+    <row r="22" spans="1:50" s="20" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="94"/>
+      <c r="B22" s="94" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="20" t="s">
@@ -7477,11 +7774,23 @@
       <c r="AQ22" s="66"/>
       <c r="AR22" s="66"/>
       <c r="AS22" s="66"/>
+      <c r="AV22" s="42">
+        <f>Q22/(F22/(F22+16))</f>
+        <v>4608</v>
+      </c>
+      <c r="AW22" s="42">
+        <f t="shared" si="4"/>
+        <v>5120</v>
+      </c>
+      <c r="AX22" s="42">
+        <f t="shared" si="5"/>
+        <v>4352</v>
+      </c>
     </row>
-    <row r="23" spans="1:45" s="20" customFormat="1" ht="61.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="107"/>
-      <c r="B23" s="107"/>
-      <c r="C23" s="107" t="s">
+    <row r="23" spans="1:50" s="20" customFormat="1" ht="61.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="94"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="94" t="s">
         <v>15</v>
       </c>
       <c r="D23" s="20">
@@ -7581,11 +7890,23 @@
       <c r="AQ23" s="66"/>
       <c r="AR23" s="66"/>
       <c r="AS23" s="66"/>
+      <c r="AV23" s="42">
+        <f>Q23/(F23/(F23+16))</f>
+        <v>2176</v>
+      </c>
+      <c r="AW23" s="42">
+        <f t="shared" si="4"/>
+        <v>2304</v>
+      </c>
+      <c r="AX23" s="42">
+        <f t="shared" si="5"/>
+        <v>2112</v>
+      </c>
     </row>
-    <row r="24" spans="1:45" s="20" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="107"/>
-      <c r="B24" s="107"/>
-      <c r="C24" s="107"/>
+    <row r="24" spans="1:50" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="94"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="94"/>
       <c r="D24" s="20">
         <v>128</v>
       </c>
@@ -7617,7 +7938,7 @@
         <v>192</v>
       </c>
       <c r="M24" s="12">
-        <f t="shared" ref="M24:M37" si="4">D24*F24/1024</f>
+        <f t="shared" ref="M24:M37" si="6">D24*F24/1024</f>
         <v>8</v>
       </c>
       <c r="N24" s="23">
@@ -7683,11 +8004,23 @@
       <c r="AQ24" s="66"/>
       <c r="AR24" s="66"/>
       <c r="AS24" s="66"/>
+      <c r="AV24" s="42">
+        <f>Q24/(F24/(F24+16))</f>
+        <v>2560</v>
+      </c>
+      <c r="AW24" s="42">
+        <f t="shared" si="4"/>
+        <v>3072</v>
+      </c>
+      <c r="AX24" s="42">
+        <f t="shared" si="5"/>
+        <v>2304</v>
+      </c>
     </row>
-    <row r="25" spans="1:45" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A25" s="107"/>
-      <c r="B25" s="107"/>
-      <c r="C25" s="107"/>
+    <row r="25" spans="1:50" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A25" s="94"/>
+      <c r="B25" s="94"/>
+      <c r="C25" s="94"/>
       <c r="D25" s="20">
         <v>128</v>
       </c>
@@ -7719,7 +8052,7 @@
         <v>768</v>
       </c>
       <c r="M25" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="N25" s="23">
@@ -7785,9 +8118,21 @@
       <c r="AQ25" s="66"/>
       <c r="AR25" s="66"/>
       <c r="AS25" s="66"/>
+      <c r="AV25" s="42">
+        <f>Q25/(F25/(F25+16))</f>
+        <v>8704</v>
+      </c>
+      <c r="AW25" s="42">
+        <f t="shared" si="4"/>
+        <v>9216</v>
+      </c>
+      <c r="AX25" s="42">
+        <f t="shared" si="5"/>
+        <v>8448</v>
+      </c>
     </row>
-    <row r="26" spans="1:45" s="30" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="106"/>
+    <row r="26" spans="1:50" s="30" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A26" s="112"/>
       <c r="B26" s="30" t="s">
         <v>16</v>
       </c>
@@ -7816,13 +8161,21 @@
       <c r="M26" s="32"/>
       <c r="N26" s="33"/>
       <c r="O26" s="32"/>
+      <c r="AW26" s="42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AX26" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:45" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="108"/>
-      <c r="B27" s="110" t="s">
+    <row r="27" spans="1:50" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="99"/>
+      <c r="B27" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="108" t="s">
+      <c r="C27" s="99" t="s">
         <v>15</v>
       </c>
       <c r="D27" s="24">
@@ -7856,7 +8209,7 @@
         <v>32</v>
       </c>
       <c r="M27" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="N27" s="28">
@@ -7899,11 +8252,23 @@
       <c r="AQ27" s="67"/>
       <c r="AR27" s="67"/>
       <c r="AS27" s="67"/>
+      <c r="AV27" s="42">
+        <f t="shared" ref="AV27:AV29" si="7">Q27/(F27/(F27+16))</f>
+        <v>2176</v>
+      </c>
+      <c r="AW27" s="42">
+        <f t="shared" si="4"/>
+        <v>2304</v>
+      </c>
+      <c r="AX27" s="42">
+        <f t="shared" si="5"/>
+        <v>2112</v>
+      </c>
     </row>
-    <row r="28" spans="1:45" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="108"/>
-      <c r="B28" s="108"/>
-      <c r="C28" s="108"/>
+    <row r="28" spans="1:50" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="99"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="99"/>
       <c r="D28" s="24">
         <v>128</v>
       </c>
@@ -7935,7 +8300,7 @@
         <v>8</v>
       </c>
       <c r="M28" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="N28" s="28">
@@ -7978,11 +8343,23 @@
       <c r="AQ28" s="67"/>
       <c r="AR28" s="67"/>
       <c r="AS28" s="67"/>
+      <c r="AV28" s="42">
+        <f t="shared" si="7"/>
+        <v>2560</v>
+      </c>
+      <c r="AW28" s="42">
+        <f t="shared" si="4"/>
+        <v>3072</v>
+      </c>
+      <c r="AX28" s="42">
+        <f t="shared" si="5"/>
+        <v>2304</v>
+      </c>
     </row>
-    <row r="29" spans="1:45" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="108"/>
-      <c r="B29" s="108"/>
-      <c r="C29" s="108"/>
+    <row r="29" spans="1:50" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="99"/>
+      <c r="B29" s="99"/>
+      <c r="C29" s="99"/>
       <c r="D29" s="24">
         <v>128</v>
       </c>
@@ -8014,7 +8391,7 @@
         <v>32</v>
       </c>
       <c r="M29" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="N29" s="28">
@@ -8057,12 +8434,24 @@
       <c r="AQ29" s="67"/>
       <c r="AR29" s="67"/>
       <c r="AS29" s="67"/>
+      <c r="AV29" s="42">
+        <f t="shared" si="7"/>
+        <v>8704</v>
+      </c>
+      <c r="AW29" s="42">
+        <f t="shared" si="4"/>
+        <v>9216</v>
+      </c>
+      <c r="AX29" s="42">
+        <f t="shared" si="5"/>
+        <v>8448</v>
+      </c>
     </row>
-    <row r="30" spans="1:45" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="106" t="s">
+    <row r="30" spans="1:50" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="109" t="s">
+      <c r="B30" s="95" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="13" t="s">
@@ -8099,7 +8488,7 @@
         <v>0.375</v>
       </c>
       <c r="M30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.375</v>
       </c>
       <c r="N30" s="16"/>
@@ -8146,10 +8535,18 @@
       <c r="AQ30" s="68"/>
       <c r="AR30" s="68"/>
       <c r="AS30" s="68"/>
+      <c r="AW30" s="42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AX30" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:45" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="106"/>
-      <c r="B31" s="109"/>
+    <row r="31" spans="1:50" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="112"/>
+      <c r="B31" s="95"/>
       <c r="C31" s="13" t="s">
         <v>12</v>
       </c>
@@ -8184,7 +8581,7 @@
         <v>0.1875</v>
       </c>
       <c r="M31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.1875</v>
       </c>
       <c r="N31" s="16"/>
@@ -8233,10 +8630,18 @@
       </c>
       <c r="AR31" s="68"/>
       <c r="AS31" s="68"/>
+      <c r="AW31" s="42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AX31" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:45" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A32" s="107"/>
-      <c r="B32" s="107" t="s">
+    <row r="32" spans="1:50" s="20" customFormat="1" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="94"/>
+      <c r="B32" s="94" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="20" t="s">
@@ -8273,7 +8678,7 @@
         <v>384</v>
       </c>
       <c r="M32" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="N32" s="23">
@@ -8335,11 +8740,23 @@
       <c r="AQ32" s="66"/>
       <c r="AR32" s="66"/>
       <c r="AS32" s="66"/>
+      <c r="AV32" s="42">
+        <f t="shared" ref="AV32:AV34" si="8">Q32/(F32/(F32+16))</f>
+        <v>4352</v>
+      </c>
+      <c r="AW32" s="42">
+        <f t="shared" si="4"/>
+        <v>4608</v>
+      </c>
+      <c r="AX32" s="42">
+        <f t="shared" si="5"/>
+        <v>4224</v>
+      </c>
     </row>
-    <row r="33" spans="1:45" s="20" customFormat="1" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="107"/>
-      <c r="B33" s="107"/>
-      <c r="C33" s="107" t="s">
+    <row r="33" spans="1:50" s="20" customFormat="1" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="94"/>
+      <c r="B33" s="94"/>
+      <c r="C33" s="94" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="20">
@@ -8373,7 +8790,7 @@
         <v>384</v>
       </c>
       <c r="M33" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="N33" s="23">
@@ -8435,11 +8852,23 @@
       <c r="AQ33" s="66"/>
       <c r="AR33" s="66"/>
       <c r="AS33" s="66"/>
+      <c r="AV33" s="42">
+        <f t="shared" si="8"/>
+        <v>1088</v>
+      </c>
+      <c r="AW33" s="42">
+        <f t="shared" si="4"/>
+        <v>1152</v>
+      </c>
+      <c r="AX33" s="42">
+        <f t="shared" si="5"/>
+        <v>1056</v>
+      </c>
     </row>
-    <row r="34" spans="1:45" s="20" customFormat="1" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="107"/>
-      <c r="B34" s="107"/>
-      <c r="C34" s="107"/>
+    <row r="34" spans="1:50" s="20" customFormat="1" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="94"/>
+      <c r="B34" s="94"/>
+      <c r="C34" s="94"/>
       <c r="D34" s="20">
         <v>64</v>
       </c>
@@ -8471,7 +8900,7 @@
         <v>96</v>
       </c>
       <c r="M34" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N34" s="23">
@@ -8537,9 +8966,21 @@
       <c r="AQ34" s="66"/>
       <c r="AR34" s="66"/>
       <c r="AS34" s="66"/>
+      <c r="AV34" s="42">
+        <f t="shared" si="8"/>
+        <v>1280</v>
+      </c>
+      <c r="AW34" s="42">
+        <f t="shared" si="4"/>
+        <v>1536</v>
+      </c>
+      <c r="AX34" s="42">
+        <f t="shared" si="5"/>
+        <v>1152</v>
+      </c>
     </row>
-    <row r="35" spans="1:45" s="30" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A35" s="106"/>
+    <row r="35" spans="1:50" s="30" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A35" s="112"/>
       <c r="B35" s="30" t="s">
         <v>16</v>
       </c>
@@ -8569,13 +9010,21 @@
       <c r="N35" s="33"/>
       <c r="O35" s="32"/>
       <c r="AL35" s="90"/>
+      <c r="AW35" s="42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AX35" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:45" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="108"/>
-      <c r="B36" s="108" t="s">
+    <row r="36" spans="1:50" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="99"/>
+      <c r="B36" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="108" t="s">
+      <c r="C36" s="99" t="s">
         <v>15</v>
       </c>
       <c r="D36" s="24">
@@ -8609,7 +9058,7 @@
         <v>16</v>
       </c>
       <c r="M36" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="N36" s="28">
@@ -8666,11 +9115,23 @@
       <c r="AQ36" s="67"/>
       <c r="AR36" s="67"/>
       <c r="AS36" s="67"/>
+      <c r="AV36" s="42">
+        <f t="shared" ref="AV36:AV37" si="9">Q36/(F36/(F36+16))</f>
+        <v>1088</v>
+      </c>
+      <c r="AW36" s="42">
+        <f t="shared" si="4"/>
+        <v>1152</v>
+      </c>
+      <c r="AX36" s="42">
+        <f t="shared" si="5"/>
+        <v>1056</v>
+      </c>
     </row>
-    <row r="37" spans="1:45" s="24" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="108"/>
-      <c r="B37" s="108"/>
-      <c r="C37" s="108"/>
+    <row r="37" spans="1:50" s="24" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="99"/>
+      <c r="B37" s="99"/>
+      <c r="C37" s="99"/>
       <c r="D37" s="24">
         <v>64</v>
       </c>
@@ -8702,7 +9163,7 @@
         <v>4</v>
       </c>
       <c r="M37" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N37" s="28">
@@ -8763,12 +9224,24 @@
       <c r="AQ37" s="67"/>
       <c r="AR37" s="67"/>
       <c r="AS37" s="67"/>
+      <c r="AV37" s="42">
+        <f t="shared" si="9"/>
+        <v>1280</v>
+      </c>
+      <c r="AW37" s="42">
+        <f t="shared" si="4"/>
+        <v>1536</v>
+      </c>
+      <c r="AX37" s="42">
+        <f t="shared" si="5"/>
+        <v>1152</v>
+      </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A38" s="95" t="s">
+    <row r="38" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A38" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="96"/>
+      <c r="B38" s="102"/>
       <c r="C38" s="3" t="s">
         <v>17</v>
       </c>
@@ -8791,9 +9264,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="39" spans="1:45" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="97"/>
-      <c r="B39" s="98"/>
+    <row r="39" spans="1:50" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="113"/>
+      <c r="B39" s="114"/>
       <c r="C39" s="30" t="s">
         <v>27</v>
       </c>
@@ -8844,9 +9317,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:45" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="97"/>
-      <c r="B40" s="98"/>
+    <row r="40" spans="1:50" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="113"/>
+      <c r="B40" s="114"/>
       <c r="C40" s="30" t="s">
         <v>28</v>
       </c>
@@ -8881,9 +9354,9 @@
       <c r="N40" s="33"/>
       <c r="O40" s="32"/>
     </row>
-    <row r="41" spans="1:45" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="97"/>
-      <c r="B41" s="98"/>
+    <row r="41" spans="1:50" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="113"/>
+      <c r="B41" s="114"/>
       <c r="C41" s="30" t="s">
         <v>29</v>
       </c>
@@ -8934,9 +9407,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:45" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="97"/>
-      <c r="B42" s="98"/>
+    <row r="42" spans="1:50" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="113"/>
+      <c r="B42" s="114"/>
       <c r="C42" s="30" t="s">
         <v>28</v>
       </c>
@@ -8971,9 +9444,9 @@
       <c r="N42" s="33"/>
       <c r="O42" s="32"/>
     </row>
-    <row r="43" spans="1:45" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="99"/>
-      <c r="B43" s="100"/>
+    <row r="43" spans="1:50" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="115"/>
+      <c r="B43" s="116"/>
       <c r="C43" s="30" t="s">
         <v>30</v>
       </c>
@@ -9024,7 +9497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:45" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:50" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
@@ -9035,7 +9508,7 @@
         <v>5862.5625</v>
       </c>
       <c r="N44" s="8">
-        <f t="shared" ref="N44:S44" si="5">SUM(N3:N43)</f>
+        <f t="shared" ref="N44:S44" si="10">SUM(N3:N43)</f>
         <v>579.09375</v>
       </c>
       <c r="O44" s="8">
@@ -9043,19 +9516,19 @@
         <v>488.7890625</v>
       </c>
       <c r="P44" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>705829</v>
       </c>
       <c r="Q44" s="76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>46373</v>
       </c>
       <c r="R44" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>850</v>
       </c>
       <c r="S44" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>9180</v>
       </c>
       <c r="U44" s="8">
@@ -9076,8 +9549,20 @@
       <c r="AL44" s="63"/>
       <c r="AM44" s="63"/>
       <c r="AN44" s="63"/>
+      <c r="AV44" s="8">
+        <f>SUM(AV3:AV43)</f>
+        <v>53984</v>
+      </c>
+      <c r="AW44" s="8">
+        <f>SUM(AW3:AW43)</f>
+        <v>61792</v>
+      </c>
+      <c r="AX44" s="8">
+        <f>SUM(AX3:AX43)</f>
+        <v>50080</v>
+      </c>
     </row>
-    <row r="45" spans="1:45" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:50" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="38"/>
       <c r="C45" s="38"/>
       <c r="L45" s="39"/>
@@ -9097,36 +9582,28 @@
       <c r="AL45" s="77"/>
       <c r="AM45" s="77"/>
       <c r="AN45" s="77"/>
+      <c r="AV45" s="37">
+        <f>AV44/Q44</f>
+        <v>1.1641256765790438</v>
+      </c>
+      <c r="AW45" s="37">
+        <f>AW44/Q44</f>
+        <v>1.332499514803873</v>
+      </c>
+      <c r="AX45" s="37">
+        <f>AX44/Q44</f>
+        <v>1.0799387574666293</v>
+      </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:50" x14ac:dyDescent="0.25">
       <c r="Q46" s="47">
         <f>Q45/Q44</f>
         <v>0.37539085243568454</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="AG1:AI1"/>
-    <mergeCell ref="AA1:AF1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AN1"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A20:A29"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A30:A37"/>
-    <mergeCell ref="B22:B25"/>
+  <mergeCells count="38">
+    <mergeCell ref="AV1:AW1"/>
     <mergeCell ref="AQ1:AS1"/>
     <mergeCell ref="A38:B43"/>
     <mergeCell ref="A3:B3"/>
@@ -9143,6 +9620,27 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A20:A29"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A30:A37"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="AG1:AI1"/>
+    <mergeCell ref="AA1:AF1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AN1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>